<commit_message>
fix: Excel sheet updated
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deep Soni\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deep Soni\Desktop\petshop-desire\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
   <si>
     <t>Module</t>
   </si>
@@ -74,9 +74,6 @@
     <t>2. Shop</t>
   </si>
   <si>
-    <t>brandName</t>
-  </si>
-  <si>
     <t>userId - ref</t>
   </si>
   <si>
@@ -167,7 +164,7 @@
     <t>Owner</t>
   </si>
   <si>
-    <t>userId</t>
+    <t>shopId</t>
   </si>
 </sst>
 </file>
@@ -494,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C26" sqref="A1:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,7 +574,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -585,31 +582,31 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
         <v>39</v>
-      </c>
-      <c r="C12" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -617,15 +614,15 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
         <v>41</v>
-      </c>
-      <c r="C16" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>4</v>
@@ -636,23 +633,23 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
         <v>43</v>
-      </c>
-      <c r="C20" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -660,7 +657,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
@@ -668,7 +665,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
@@ -676,7 +673,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -684,20 +681,20 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" t="s">
         <v>46</v>
-      </c>
-      <c r="C26" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>
@@ -708,7 +705,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
@@ -716,7 +713,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C30" t="s">
         <v>9</v>
@@ -724,7 +721,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
@@ -732,7 +729,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
@@ -740,10 +737,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" t="s">
         <v>31</v>
-      </c>
-      <c r="B34" t="s">
-        <v>32</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
@@ -751,26 +748,26 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" t="s">
         <v>33</v>
-      </c>
-      <c r="C35" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" t="s">
         <v>36</v>
-      </c>
-      <c r="C37" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
learn: reference relation, shop apis, populate, api integration in react
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C26" sqref="A1:C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>